<commit_message>
- add generation for: Valves, Analog Input/Output, Discrete Input/Output
</commit_message>
<xml_diff>
--- a/src/main/resources/sources/devices.xlsx
+++ b/src/main/resources/sources/devices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enere\IdeaProjects\alarmsGen\src\main\resources\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enere\IdeaProjects\genCodePLCopenXML\src\main\resources\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD914BD6-228A-4DAF-9D51-6FF5197DC2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC7AC36-B3A0-4D2A-9B62-6CF1A2F4506D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="4140" windowWidth="28800" windowHeight="15345" xr2:uid="{1226FF66-870F-4237-90F5-6B5DC0EF370E}"/>
+    <workbookView xWindow="9030" yWindow="4050" windowWidth="28800" windowHeight="15345" xr2:uid="{1226FF66-870F-4237-90F5-6B5DC0EF370E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
   <si>
     <t>Motor</t>
   </si>
@@ -153,6 +153,213 @@
   </si>
   <si>
     <t>мда</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>A15.DO11</t>
+  </si>
+  <si>
+    <t>A15.DO13</t>
+  </si>
+  <si>
+    <t>A15.DO14</t>
+  </si>
+  <si>
+    <t>клапан пидора</t>
+  </si>
+  <si>
+    <t>клапан шлюхи</t>
+  </si>
+  <si>
+    <t>клапан заказчика</t>
+  </si>
+  <si>
+    <t>клапан хуйла</t>
+  </si>
+  <si>
+    <t>Клапан А1</t>
+  </si>
+  <si>
+    <t>Клапан А3</t>
+  </si>
+  <si>
+    <t>Клапан А4</t>
+  </si>
+  <si>
+    <t>Клапан А2</t>
+  </si>
+  <si>
+    <t>V_A_1</t>
+  </si>
+  <si>
+    <t>V_A_2</t>
+  </si>
+  <si>
+    <t>V_A_3</t>
+  </si>
+  <si>
+    <t>V_A_4</t>
+  </si>
+  <si>
+    <t>Analog Input</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Давлние PE 1</t>
+  </si>
+  <si>
+    <t>PE_1</t>
+  </si>
+  <si>
+    <t>A10.AI1</t>
+  </si>
+  <si>
+    <t>Давлние PE 2</t>
+  </si>
+  <si>
+    <t>PE_2</t>
+  </si>
+  <si>
+    <t>A11.AI1</t>
+  </si>
+  <si>
+    <t>Давление в очке</t>
+  </si>
+  <si>
+    <t>Давление вне очка</t>
+  </si>
+  <si>
+    <t>Analog Output</t>
+  </si>
+  <si>
+    <t>Скорость UZ 1</t>
+  </si>
+  <si>
+    <t>Скорость UZ 2</t>
+  </si>
+  <si>
+    <t>sp_UZ_1</t>
+  </si>
+  <si>
+    <t>sp_UZ_2</t>
+  </si>
+  <si>
+    <t>A4.AI14</t>
+  </si>
+  <si>
+    <t>A4.AI13</t>
+  </si>
+  <si>
+    <t>Скорость горения очка</t>
+  </si>
+  <si>
+    <t>Расход воды на тушение очка</t>
+  </si>
+  <si>
+    <t>out real</t>
+  </si>
+  <si>
+    <t>out int</t>
+  </si>
+  <si>
+    <t>Discrete Input</t>
+  </si>
+  <si>
+    <t>keyEmergency</t>
+  </si>
+  <si>
+    <t>keyStart</t>
+  </si>
+  <si>
+    <t>keyStop</t>
+  </si>
+  <si>
+    <t>keyReset</t>
+  </si>
+  <si>
+    <t>Emergency Stop</t>
+  </si>
+  <si>
+    <t>Start process</t>
+  </si>
+  <si>
+    <t>Stop process</t>
+  </si>
+  <si>
+    <t>Reset alamrs</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Key - start auto mode</t>
+  </si>
+  <si>
+    <t>Key - stop auto mode</t>
+  </si>
+  <si>
+    <t>Key - reset alarms</t>
+  </si>
+  <si>
+    <t>Key - emergency stop</t>
+  </si>
+  <si>
+    <t>Discrete Output</t>
+  </si>
+  <si>
+    <t>ledWhite</t>
+  </si>
+  <si>
+    <t>ledGreen</t>
+  </si>
+  <si>
+    <t>ledYellow</t>
+  </si>
+  <si>
+    <t>ledRed</t>
+  </si>
+  <si>
+    <t>cmdSiren</t>
+  </si>
+  <si>
+    <t>ready to work</t>
+  </si>
+  <si>
+    <t>system in operation</t>
+  </si>
+  <si>
+    <t>system in standby mode</t>
+  </si>
+  <si>
+    <t>there is at least one alarm in the system</t>
+  </si>
+  <si>
+    <t>new alarm notification</t>
+  </si>
+  <si>
+    <t>Lamp state - white - ready to work</t>
+  </si>
+  <si>
+    <t>Lamp state - green - system in operation</t>
+  </si>
+  <si>
+    <t>Lamp state - yellow - system in standby mode</t>
+  </si>
+  <si>
+    <t>Lamp state - red - there is at least one alarm in the system</t>
+  </si>
+  <si>
+    <t>Command - sound siren - new alarm notification</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -478,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E22D66C-7172-41DC-8C4F-63F2081667A9}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,6 +846,438 @@
         <v>39</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13"/>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14"/>
+      <c r="H14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15"/>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16"/>
+      <c r="H16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23"/>
+      <c r="H23" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="D30"/>
+      <c r="J30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33"/>
+      <c r="J33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="J35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="2">
+        <v>4</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="J36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="2">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>